<commit_message>
ver 35.1 Final Version of the SailTimer Windex branch
</commit_message>
<xml_diff>
--- a/VariousAppDevelopmentAssets/TWD_raw.xlsx
+++ b/VariousAppDevelopmentAssets/TWD_raw.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VolkerPetersen\Dropbox\ProgramCode\Android\SailingRace\VariousAppDevelopmentAssets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E6DEAEA6-E0EF-4F71-BA08-318EC2F57CFC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="19320" windowHeight="7755"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="19320" windowHeight="7755" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Real Data</t>
   </si>
@@ -32,13 +38,45 @@
   <si>
     <t>Chart showing 1 hour rolling avg (orange) vs. 5 min rolling avg with +/- 1 StdDev of 1 hour rolling avg.</t>
   </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>LP-X</t>
+  </si>
+  <si>
+    <t>LP-Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alpha = </t>
+  </si>
+  <si>
+    <t>Raw</t>
+  </si>
+  <si>
+    <t>Filtered</t>
+  </si>
+  <si>
+    <t>raw_360</t>
+  </si>
+  <si>
+    <t>lpf_360</t>
+  </si>
+  <si>
+    <t>kal_360</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -85,23 +123,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -115,8 +154,1384 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>raw_360</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$3:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$3:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>363</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>366</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>361</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>353</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>356</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>361</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>361</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>353</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>369</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>358</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>369</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>351</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>354</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>361</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>365</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F13F-4F85-9562-04DC55F958ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>lpf_360</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$3:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$3:$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>363.75059523917491</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>363.56284793741418</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>364.17231912861018</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>363.37904429618385</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>360.78820381099376</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>359.58842019866717</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>359.94219483745576</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>362.45667432558656</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>361.8403481221589</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>361.62966553427782</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>359.47067203516707</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>361.85653418192805</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>360.88846872852207</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>362.92108597638719</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>359.93665688783392</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>358.44437742312419</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>359.08662633807518</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>359.3159144658909</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>360.74050930090795</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F13F-4F85-9562-04DC55F958ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>kal_360</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$3:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$3:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>362.33</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>362.55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>363.45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>362.91</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>361.089</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>360.18360000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>360.31630000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>361.68</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>361.44400000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>360.82490000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>359.92200000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>360.97739999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>360.6232</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>361.553</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>360.36320000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>359.61099999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>359.77</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>359.79700000000003</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>360.29880000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F13F-4F85-9562-04DC55F958ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="536254672"/>
+        <c:axId val="536256640"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="536254672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="536256640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="536256640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="536254672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -136,7 +1551,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -157,6 +1578,47 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>604837</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>300037</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB2C3268-26CE-4C7B-BD3C-7D16AABBE3AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -205,7 +1667,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -238,9 +1700,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -273,6 +1752,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -448,11 +1944,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3393"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37771,7 +39267,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4:C3393">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$T4=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -37781,19 +39277,1022 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>E3</f>
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>365</v>
+      </c>
+      <c r="C3" s="7">
+        <f>IF(L3&lt;300,L3+360,L3)</f>
+        <v>365</v>
+      </c>
+      <c r="D3" s="7">
+        <f>IF(K3&lt;300,K3+360,K3)</f>
+        <v>365</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6">
+        <f>MOD(B3,360)</f>
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <f>COS(RADIANS(F3))</f>
+        <v>0.99619469809174555</v>
+      </c>
+      <c r="H3">
+        <f>SIN(RADIANS(F3))</f>
+        <v>8.7155742747658166E-2</v>
+      </c>
+      <c r="I3">
+        <f>G3</f>
+        <v>0.99619469809174555</v>
+      </c>
+      <c r="J3">
+        <f>H3</f>
+        <v>8.7155742747658166E-2</v>
+      </c>
+      <c r="K3" s="7">
+        <f>MOD(DEGREES(ATAN2(I3,J3))+360, 360)</f>
+        <v>5</v>
+      </c>
+      <c r="L3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A22" si="0">E4</f>
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>360</v>
+      </c>
+      <c r="C4" s="7">
+        <f t="shared" ref="C4:C22" si="1">IF(L4&lt;300,L4+360,L4)</f>
+        <v>362.33</v>
+      </c>
+      <c r="D4" s="7">
+        <f t="shared" ref="D4:D22" si="2">IF(K4&lt;300,K4+360,K4)</f>
+        <v>363.75059523917491</v>
+      </c>
+      <c r="E4">
+        <f>E3+1</f>
+        <v>2</v>
+      </c>
+      <c r="F4" s="6">
+        <f t="shared" ref="F4:F22" si="3">MOD(B4,360)</f>
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G22" si="4">COS(RADIANS(F4))</f>
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H22" si="5">SIN(RADIANS(F4))</f>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f>G4*$J$1+I3*(1-$J$1)</f>
+        <v>0.99714602356880921</v>
+      </c>
+      <c r="J4">
+        <f>H4*$J$1+J3*(1-$J$1)</f>
+        <v>6.5366807060743631E-2</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" ref="K4:K22" si="6">MOD(DEGREES(ATAN2(I4,J4))+360, 360)</f>
+        <v>3.7505952391749133</v>
+      </c>
+      <c r="L4">
+        <v>2.33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>363</v>
+      </c>
+      <c r="C5" s="7">
+        <f t="shared" si="1"/>
+        <v>362.55</v>
+      </c>
+      <c r="D5" s="7">
+        <f t="shared" si="2"/>
+        <v>363.56284793741418</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E22" si="7">E4+1</f>
+        <v>3</v>
+      </c>
+      <c r="F5" s="6">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="4"/>
+        <v>0.99862953475457383</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="5"/>
+        <v>5.2335956242943835E-2</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I22" si="8">G5*$J$1+I4*(1-$J$1)</f>
+        <v>0.9975169013652504</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5:J22" si="9">H5*$J$1+J4*(1-$J$1)</f>
+        <v>6.2109094356293679E-2</v>
+      </c>
+      <c r="K5" s="7">
+        <f t="shared" si="6"/>
+        <v>3.5628479374141762</v>
+      </c>
+      <c r="L5">
+        <v>2.5499999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>366</v>
+      </c>
+      <c r="C6" s="7">
+        <f t="shared" si="1"/>
+        <v>363.45</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" si="2"/>
+        <v>364.17231912861018</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="F6" s="6">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="4"/>
+        <v>0.99452189536827329</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="5"/>
+        <v>0.10452846326765347</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="8"/>
+        <v>0.99676814986600615</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="9"/>
+        <v>7.2713936584133623E-2</v>
+      </c>
+      <c r="K6" s="7">
+        <f t="shared" si="6"/>
+        <v>4.1723191286101837</v>
+      </c>
+      <c r="L6">
+        <v>3.45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>361</v>
+      </c>
+      <c r="C7" s="7">
+        <f t="shared" si="1"/>
+        <v>362.91</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" si="2"/>
+        <v>363.37904429618385</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="F7" s="6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="4"/>
+        <v>0.99984769515639127</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="5"/>
+        <v>1.7452406437283512E-2</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="8"/>
+        <v>0.99753803618860237</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="9"/>
+        <v>5.8898554047421101E-2</v>
+      </c>
+      <c r="K7" s="7">
+        <f t="shared" si="6"/>
+        <v>3.3790442961838494</v>
+      </c>
+      <c r="L7">
+        <v>2.91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>353</v>
+      </c>
+      <c r="C8" s="7">
+        <f t="shared" si="1"/>
+        <v>361.089</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="2"/>
+        <v>360.78820381099376</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="F8" s="6">
+        <f t="shared" si="3"/>
+        <v>353</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="4"/>
+        <v>0.99254615164132209</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="5"/>
+        <v>-0.12186934340514723</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="8"/>
+        <v>0.9962900650517823</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="9"/>
+        <v>1.3706579684279015E-2</v>
+      </c>
+      <c r="K8" s="7">
+        <f t="shared" si="6"/>
+        <v>0.78820381099376391</v>
+      </c>
+      <c r="L8">
+        <v>1.089</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>356</v>
+      </c>
+      <c r="C9" s="7">
+        <f t="shared" si="1"/>
+        <v>360.18360000000001</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" si="2"/>
+        <v>359.58842019866717</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="F9" s="6">
+        <f t="shared" si="3"/>
+        <v>356</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="4"/>
+        <v>0.9975640502598242</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="5"/>
+        <v>-6.9756473744125636E-2</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="8"/>
+        <v>0.99660856135379272</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="9"/>
+        <v>-7.1591836728221482E-3</v>
+      </c>
+      <c r="K9" s="7">
+        <f t="shared" si="6"/>
+        <v>359.58842019866717</v>
+      </c>
+      <c r="L9">
+        <v>0.18360000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>361</v>
+      </c>
+      <c r="C10" s="7">
+        <f t="shared" si="1"/>
+        <v>360.31630000000001</v>
+      </c>
+      <c r="D10" s="7">
+        <f t="shared" si="2"/>
+        <v>359.94219483745576</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="F10" s="6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="4"/>
+        <v>0.99984769515639127</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="5"/>
+        <v>1.7452406437283512E-2</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="8"/>
+        <v>0.99741834480444225</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="9"/>
+        <v>-1.0062861452957332E-3</v>
+      </c>
+      <c r="K10" s="7">
+        <f t="shared" si="6"/>
+        <v>359.94219483745576</v>
+      </c>
+      <c r="L10">
+        <v>0.31630000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>370</v>
+      </c>
+      <c r="C11" s="7">
+        <f t="shared" si="1"/>
+        <v>361.68</v>
+      </c>
+      <c r="D11" s="7">
+        <f t="shared" si="2"/>
+        <v>362.45667432558656</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="F11" s="6">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="4"/>
+        <v>0.98480775301220802</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="5"/>
+        <v>0.17364817766693033</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="8"/>
+        <v>0.99426569685638366</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="9"/>
+        <v>4.2657329807760783E-2</v>
+      </c>
+      <c r="K11" s="7">
+        <f t="shared" si="6"/>
+        <v>2.4566743255865617</v>
+      </c>
+      <c r="L11">
+        <v>1.68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>360</v>
+      </c>
+      <c r="C12" s="7">
+        <f t="shared" si="1"/>
+        <v>361.44400000000002</v>
+      </c>
+      <c r="D12" s="7">
+        <f t="shared" si="2"/>
+        <v>361.8403481221589</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="F12" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="8"/>
+        <v>0.99569927264228775</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="9"/>
+        <v>3.199299735582059E-2</v>
+      </c>
+      <c r="K12" s="7">
+        <f t="shared" si="6"/>
+        <v>1.8403481221589004</v>
+      </c>
+      <c r="L12">
+        <v>1.444</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>361</v>
+      </c>
+      <c r="C13" s="7">
+        <f t="shared" si="1"/>
+        <v>360.82490000000001</v>
+      </c>
+      <c r="D13" s="7">
+        <f t="shared" si="2"/>
+        <v>361.62966553427782</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+      <c r="F13" s="6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="4"/>
+        <v>0.99984769515639127</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="5"/>
+        <v>1.7452406437283512E-2</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="8"/>
+        <v>0.99673637827081363</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="9"/>
+        <v>2.8357849626186322E-2</v>
+      </c>
+      <c r="K13" s="7">
+        <f t="shared" si="6"/>
+        <v>1.6296655342778195</v>
+      </c>
+      <c r="L13">
+        <v>0.82489999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>353</v>
+      </c>
+      <c r="C14" s="7">
+        <f t="shared" si="1"/>
+        <v>359.92200000000003</v>
+      </c>
+      <c r="D14" s="7">
+        <f t="shared" si="2"/>
+        <v>359.47067203516707</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="7"/>
+        <v>12</v>
+      </c>
+      <c r="F14" s="6">
+        <f t="shared" si="3"/>
+        <v>353</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="4"/>
+        <v>0.99254615164132209</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="5"/>
+        <v>-0.12186934340514723</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="8"/>
+        <v>0.99568882161344074</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="9"/>
+        <v>-9.198948631647063E-3</v>
+      </c>
+      <c r="K14" s="7">
+        <f t="shared" si="6"/>
+        <v>359.47067203516707</v>
+      </c>
+      <c r="L14">
+        <v>359.92200000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>369</v>
+      </c>
+      <c r="C15" s="7">
+        <f t="shared" si="1"/>
+        <v>360.97739999999999</v>
+      </c>
+      <c r="D15" s="7">
+        <f t="shared" si="2"/>
+        <v>361.85653418192805</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="7"/>
+        <v>13</v>
+      </c>
+      <c r="F15" s="6">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="4"/>
+        <v>0.98768834059513777</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="5"/>
+        <v>0.15643446504023087</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="8"/>
+        <v>0.993688701358865</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="9"/>
+        <v>3.2209404786322421E-2</v>
+      </c>
+      <c r="K15" s="7">
+        <f t="shared" si="6"/>
+        <v>1.8565341819280547</v>
+      </c>
+      <c r="L15">
+        <v>0.97740000000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>358</v>
+      </c>
+      <c r="C16" s="7">
+        <f t="shared" si="1"/>
+        <v>360.6232</v>
+      </c>
+      <c r="D16" s="7">
+        <f t="shared" si="2"/>
+        <v>360.88846872852207</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+      <c r="F16" s="6">
+        <f t="shared" si="3"/>
+        <v>358</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="4"/>
+        <v>0.99939082701909576</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="5"/>
+        <v>-3.4899496702500823E-2</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="8"/>
+        <v>0.99511423277392275</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="9"/>
+        <v>1.543217941411661E-2</v>
+      </c>
+      <c r="K16" s="7">
+        <f t="shared" si="6"/>
+        <v>0.88846872852207071</v>
+      </c>
+      <c r="L16">
+        <v>0.62319999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>369</v>
+      </c>
+      <c r="C17" s="7">
+        <f t="shared" si="1"/>
+        <v>361.553</v>
+      </c>
+      <c r="D17" s="7">
+        <f t="shared" si="2"/>
+        <v>362.92108597638719</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="F17" s="6">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="4"/>
+        <v>0.98768834059513777</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="5"/>
+        <v>0.15643446504023087</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="8"/>
+        <v>0.99325775972922647</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="9"/>
+        <v>5.0682750820645175E-2</v>
+      </c>
+      <c r="K17" s="7">
+        <f t="shared" si="6"/>
+        <v>2.9210859763871895</v>
+      </c>
+      <c r="L17">
+        <v>1.5529999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>351</v>
+      </c>
+      <c r="C18" s="7">
+        <f t="shared" si="1"/>
+        <v>360.36320000000001</v>
+      </c>
+      <c r="D18" s="7">
+        <f t="shared" si="2"/>
+        <v>359.93665688783392</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="F18" s="6">
+        <f t="shared" si="3"/>
+        <v>351</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="4"/>
+        <v>0.98768834059513766</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="5"/>
+        <v>-0.15643446504023112</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="8"/>
+        <v>0.9918654049457043</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="9"/>
+        <v>-1.0965531445738946E-3</v>
+      </c>
+      <c r="K18" s="7">
+        <f t="shared" si="6"/>
+        <v>359.93665688783392</v>
+      </c>
+      <c r="L18">
+        <v>0.36320000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>354</v>
+      </c>
+      <c r="C19" s="7">
+        <f t="shared" si="1"/>
+        <v>359.61099999999999</v>
+      </c>
+      <c r="D19" s="7">
+        <f t="shared" si="2"/>
+        <v>358.44437742312419</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="7"/>
+        <v>17</v>
+      </c>
+      <c r="F19" s="6">
+        <f t="shared" si="3"/>
+        <v>354</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="4"/>
+        <v>0.99452189536827329</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="5"/>
+        <v>-0.10452846326765342</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="8"/>
+        <v>0.9925295275513466</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="9"/>
+        <v>-2.6954530675343775E-2</v>
+      </c>
+      <c r="K19" s="7">
+        <f t="shared" si="6"/>
+        <v>358.44437742312419</v>
+      </c>
+      <c r="L19">
+        <v>359.61099999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>361</v>
+      </c>
+      <c r="C20" s="7">
+        <f t="shared" si="1"/>
+        <v>359.77</v>
+      </c>
+      <c r="D20" s="7">
+        <f t="shared" si="2"/>
+        <v>359.08662633807518</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="7"/>
+        <v>18</v>
+      </c>
+      <c r="F20" s="6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="4"/>
+        <v>0.99984769515639127</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="5"/>
+        <v>1.7452406437283512E-2</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="8"/>
+        <v>0.99435906945260766</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="9"/>
+        <v>-1.5852796397186952E-2</v>
+      </c>
+      <c r="K20" s="7">
+        <f t="shared" si="6"/>
+        <v>359.08662633807518</v>
+      </c>
+      <c r="L20">
+        <v>359.77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>360</v>
+      </c>
+      <c r="C21" s="7">
+        <f t="shared" si="1"/>
+        <v>359.79700000000003</v>
+      </c>
+      <c r="D21" s="7">
+        <f t="shared" si="2"/>
+        <v>359.3159144658909</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="7"/>
+        <v>19</v>
+      </c>
+      <c r="F21" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="8"/>
+        <v>0.9957693020894558</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="9"/>
+        <v>-1.1889597297890214E-2</v>
+      </c>
+      <c r="K21" s="7">
+        <f t="shared" si="6"/>
+        <v>359.3159144658909</v>
+      </c>
+      <c r="L21">
+        <v>359.79700000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>365</v>
+      </c>
+      <c r="C22" s="7">
+        <f t="shared" si="1"/>
+        <v>360.29880000000003</v>
+      </c>
+      <c r="D22" s="7">
+        <f t="shared" si="2"/>
+        <v>360.74050930090795</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="F22" s="6">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="4"/>
+        <v>0.99619469809174555</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="5"/>
+        <v>8.7155742747658166E-2</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="8"/>
+        <v>0.99587565109002818</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="9"/>
+        <v>1.2871737713496881E-2</v>
+      </c>
+      <c r="K22" s="7">
+        <f t="shared" si="6"/>
+        <v>0.74050930090794509</v>
+      </c>
+      <c r="L22">
+        <v>0.29880000000000001</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>